<commit_message>
Tried to implement Penality Reward System (unfinished)
</commit_message>
<xml_diff>
--- a/Sufficient data/forecast_summary_B079NYQQJJ.xlsx
+++ b/Sufficient data/forecast_summary_B079NYQQJJ.xlsx
@@ -482,7 +482,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-01-05</t>
+          <t>2025-01-12</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>2</v>
@@ -522,7 +522,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-01-12</t>
+          <t>2025-01-19</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
@@ -562,7 +562,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-01-19</t>
+          <t>2025-01-26</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>2</v>
@@ -602,7 +602,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-01-26</t>
+          <t>2025-02-02</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>2</v>
@@ -642,7 +642,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-02-02</t>
+          <t>2025-02-09</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -651,7 +651,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
@@ -682,7 +682,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-02-09</t>
+          <t>2025-02-16</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>2</v>
@@ -722,7 +722,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-02-16</t>
+          <t>2025-02-23</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -731,7 +731,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
         <v>3</v>
@@ -762,7 +762,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-02-23</t>
+          <t>2025-03-02</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -771,7 +771,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>2</v>
@@ -802,7 +802,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-03-02</t>
+          <t>2025-03-09</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -811,7 +811,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>2</v>
@@ -842,7 +842,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-03-09</t>
+          <t>2025-03-16</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>3</v>
@@ -882,7 +882,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-03-16</t>
+          <t>2025-03-23</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
         <v>3</v>
@@ -922,7 +922,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-03-23</t>
+          <t>2025-03-30</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -931,7 +931,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>4</v>
@@ -962,7 +962,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
         <v>4</v>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-04-06</t>
+          <t>2025-04-13</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1011,7 +1011,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
         <v>4</v>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-20</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
         <v>4</v>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-04-20</t>
+          <t>2025-04-27</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1091,7 +1091,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
         <v>4</v>
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2022-12-25 to 2024-12-29</t>
+          <t>2022-12-25 to 2025-01-05</t>
         </is>
       </c>
     </row>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-04-13</t>
+          <t>2025-04-20</t>
         </is>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-01-05</t>
+          <t>2025-01-12</t>
         </is>
       </c>
     </row>

</xml_diff>